<commit_message>
Progress report of the Week
</commit_message>
<xml_diff>
--- a/Team Progress.xlsx
+++ b/Team Progress.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" tabRatio="640" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" tabRatio="640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week #1" sheetId="11" r:id="rId1"/>
@@ -181,25 +181,30 @@
     <t>03/04/2017 8:00 PM to 8:30 PM</t>
   </si>
   <si>
-    <t>Query Data Set to get proper Data using dataframe.js</t>
-  </si>
-  <si>
-    <t>Designed Classes in Java Script using E6</t>
-  </si>
-  <si>
-    <t>Designed UI for data selection and display various charts using HTML5 and JavaScript</t>
-  </si>
-  <si>
-    <t>Use chart.js to generate bar graphs - Running example in legacy code. Understand all fields and their functionality</t>
-  </si>
-  <si>
-    <t>Use chart.js to generate pie charts - Running example in legacy code. Understand all fields and their functionality</t>
+    <t>1) Design UI for data selection and display various charts using HTML5 and JavaScript
+2) Design model</t>
+  </si>
+  <si>
+    <t>1) Query Data Set to get proper Data using dataframe.js
+2) Design Model</t>
+  </si>
+  <si>
+    <t>1) Design Classes in Java Script using E6
+2) Sequesnce diagram</t>
+  </si>
+  <si>
+    <t>1) Use chart.js to generate bar graphs - Running example in legacy code. Understand all fields and their functionality
+2) Domain model</t>
+  </si>
+  <si>
+    <t>1) Use chart.js to generate pie charts - Running example in legacy code. Understand all fields and their functionality
+2)Domain model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,6 +428,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -458,6 +480,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -640,18 +679,18 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="109.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="109.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -674,7 +713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -697,7 +736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>24</v>
       </c>
@@ -718,7 +757,7 @@
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
@@ -737,7 +776,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
@@ -756,7 +795,7 @@
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
@@ -775,7 +814,7 @@
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -784,7 +823,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -793,7 +832,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -802,7 +841,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -811,7 +850,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -820,7 +859,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -843,18 +882,18 @@
       <selection activeCell="F3" sqref="F3:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="56.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -877,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -900,7 +939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>22</v>
       </c>
@@ -921,7 +960,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
@@ -942,7 +981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
@@ -961,7 +1000,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
@@ -980,12 +1019,12 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
@@ -1031,7 +1070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
@@ -1052,7 +1091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="9" t="s">
         <v>9</v>
@@ -1071,7 +1110,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="9" t="s">
         <v>10</v>
@@ -1090,7 +1129,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="9" t="s">
         <v>11</v>
@@ -1123,18 +1162,18 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="52.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1157,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
@@ -1178,7 +1217,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>33</v>
       </c>
@@ -1199,7 +1238,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
@@ -1220,7 +1259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
@@ -1239,7 +1278,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
@@ -1274,18 +1313,18 @@
       <selection activeCell="G15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="52.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1308,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>45</v>
       </c>
@@ -1329,7 +1368,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>33</v>
       </c>
@@ -1350,7 +1389,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
@@ -1369,7 +1408,7 @@
       </c>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
@@ -1388,7 +1427,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
@@ -1417,21 +1456,21 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="52.44140625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
@@ -1465,7 +1504,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3">
         <v>42800</v>
@@ -1473,7 +1512,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>33</v>
       </c>
@@ -1484,7 +1523,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" s="3">
         <v>42800</v>
@@ -1492,7 +1531,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
@@ -1501,7 +1540,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3">
         <v>42800</v>
@@ -1509,7 +1548,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
@@ -1526,7 +1565,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="9" t="s">
         <v>11</v>

</xml_diff>